<commit_message>
Catching exceptions of try_grandparents, Test.py fix
</commit_message>
<xml_diff>
--- a/static_files/watch.xlsx
+++ b/static_files/watch.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Code\Python\BugMiner\static_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\BugMiner\static_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{78E61F93-C561-4C60-A7A0-67FF635D7A71}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -31,12 +30,12 @@
     <definedName name="TotalDebtsLabel">#REF!</definedName>
     <definedName name="Workbook_Title">Report!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Regression</t>
   </si>
@@ -108,31 +107,37 @@
   </si>
   <si>
     <t>Failures</t>
+  </si>
+  <si>
+    <t>Delta^2</t>
+  </si>
+  <si>
+    <t>Delta^3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="66"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Century Gothic"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -140,7 +145,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1" tint="0.24994659260841701"/>
-      <name val="Century Gothic"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -221,7 +226,7 @@
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -241,6 +246,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -248,10 +258,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -262,8 +268,8 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="2" defaultTableStyle="Assets" defaultPivotStyle="PivotStyleMedium2">
-    <tableStyle name="Assets" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
-    <tableStyle name="Debts" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}"/>
+    <tableStyle name="Assets" pivot="0" count="0"/>
+    <tableStyle name="Debts" pivot="0" count="0"/>
   </tableStyles>
   <colors>
     <mruColors>
@@ -323,6 +329,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -345,7 +352,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IL"/>
+          <a:endParaRPr lang="he-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -359,14 +366,20 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Report!$B$3:$B$4</c:f>
+              <c:f>Report!$B$3:$B$6</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Regression</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Delta</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Delta^2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Delta^3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -425,6 +438,19 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -450,7 +476,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -474,19 +500,27 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Report!$C$3:$C$4</c:f>
+              <c:f>Report!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -544,7 +578,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-IL"/>
+      <a:endParaRPr lang="he-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -585,6 +619,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -597,7 +632,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Report!$B$8:$B$12</c:f>
+              <c:f>Report!$B$10:$B$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -713,7 +748,7 @@
                     </a:solidFill>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -725,12 +760,14 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Report!$C$8:$C$12</c:f>
+              <c:f>Report!$C$10:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1596,18 +1633,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor theme="5" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.88671875" style="2" customWidth="1"/>
@@ -1617,22 +1654,22 @@
     <col min="6" max="6" width="2.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="278.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="278.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="12"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1644,7 +1681,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1656,263 +1694,296 @@
       <c r="E4"/>
       <c r="F4"/>
     </row>
-    <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
       <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5">
-        <f>SUM(C3:C4)</f>
+        <f>COUNTIF(valid_bugs!B4:B119,"*Delta^2*")</f>
         <v>0</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
     </row>
-    <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5">
+        <f>COUNTIF(valid_bugs!B4:B119,"*Delta^3*")</f>
+        <v>0</v>
+      </c>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9"/>
+    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <f>SUM(C3:C6)</f>
+        <v>0</v>
+      </c>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6">
-        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Reg*", invalid_bugs!G3:G1897,"*runtime*")</f>
-        <v>0</v>
-      </c>
+    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5">
-        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*compilation*")</f>
-        <v>0</v>
-      </c>
+    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="12"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5">
-        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*runtime*")</f>
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Reg*", invalid_bugs!G3:G1897,"*runtime*")</f>
         <v>0</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>9</v>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="5">
-        <f>COUNTIFS(invalid_bugs!B2:B1896,"*Delta*", invalid_bugs!G2:G1896,"*compilation*")</f>
+        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*compilation*")</f>
         <v>0</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>16</v>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="5">
-        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*compilation*")</f>
+        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*runtime*")</f>
         <v>0</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C13" s="5">
-        <f>SUM(C8:C12)</f>
+        <f>COUNTIFS(invalid_bugs!B2:B1896,"*Delta*", invalid_bugs!G2:G1896,"*compilation*")</f>
         <v>0</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5">
+        <f>COUNTIFS(invalid_bugs!B3:B1897,"*Delta*", invalid_bugs!G3:G1897,"*compilation*")</f>
+        <v>0</v>
+      </c>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="9"/>
+    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5">
+        <f>SUM(C10:C14)</f>
+        <v>0</v>
+      </c>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3"/>
+    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3"/>
+    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="12"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="9"/>
+    <row r="20" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3"/>
+    <row r="21" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="3"/>
+    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="12"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+    <row r="24" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26"/>
+      <c r="C26"/>
+    </row>
+    <row r="27" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C28" s="3">
         <v>66.24561021495704</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
+    <row r="29" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C29" s="3">
         <v>66.24561021495704</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
+    <row r="30" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30"/>
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C32" s="3">
         <v>66.24561021495704</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
+    <row r="33" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C33" s="3">
         <v>66.24561021495704</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+    <row r="34" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C34" s="3">
         <v>67.245610214956997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <dataValidations xWindow="463" yWindow="642" count="8">
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Create a Personal Net Worth Calculator in this worksheet. Pie chart in this sheet is automatically updated based on entries in Assets and Debts worksheets" sqref="A1:A2" xr:uid="{222BE20E-6322-4369-A7A6-B3653DABF49F}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Total Assets, Total Debts, and Net Worth are automatically calculated in cells below. Pie chart is in cell E1" sqref="B1:B2 C1 B7 B15 B20 B25 B29" xr:uid="{E520F5E3-D2F5-4D91-A25F-18F200305A24}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Pie Chart starting in this cell shows percentages of Total Assets, Total Debts, and Net Worth" sqref="E1:E2" xr:uid="{7F2B811F-C931-4AEB-8497-E3AEE2C8B4B0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Debts are automatically updated in cell at right based on entries in Debts worksheet. To modify this label, update the title on the Debts worksheet" sqref="B4:B6 B11:B13" xr:uid="{C4F755A5-10D2-402D-AB11-FB827DD908C8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in this cell" sqref="C3:C6 C21:C23 C16:C18 C8:C13" xr:uid="{FB583828-508D-413F-BA05-4DC28569A1F6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in cell at right based on entries in Assets worksheet. To modify this label, update the title on the Assets worksheet" sqref="B3 B21:B23 B16:B18 B8:B10" xr:uid="{19FC26DC-1A69-4BA6-8B1F-729D9FA65BBF}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in cell at right based on entries in Assets worksheet. To modify this label, update the title on the Assets worksheet" sqref="B26:B27 B30:B32" xr:uid="{D1C6341E-8B4F-4849-BE09-E40BFCCB76A6}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in this cell" sqref="C26:C27 C30:C32" xr:uid="{2E637653-50D5-42DF-BE2B-B10F60DF8979}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Create a Personal Net Worth Calculator in this worksheet. Pie chart in this sheet is automatically updated based on entries in Assets and Debts worksheets" sqref="A1:A2"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Total Assets, Total Debts, and Net Worth are automatically calculated in cells below. Pie chart is in cell E1" sqref="B1:B2 C1 B9 B17 B22 B27 B31"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Pie Chart starting in this cell shows percentages of Total Assets, Total Debts, and Net Worth" sqref="E1:E2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Debts are automatically updated in cell at right based on entries in Debts worksheet. To modify this label, update the title on the Debts worksheet" sqref="B13:B15 B4:B8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in this cell" sqref="C3:C8 C23:C25 C18:C20 C10:C15"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in cell at right based on entries in Assets worksheet. To modify this label, update the title on the Assets worksheet" sqref="B10:B12 B23:B25 B18:B20 B3"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in cell at right based on entries in Assets worksheet. To modify this label, update the title on the Assets worksheet" sqref="B28:B29 B32:B34"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" prompt="Total Assets are automatically updated in this cell" sqref="C28:C29 C32:C34"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1925,42 +1996,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D2" sqref="A2:G118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="G46" sqref="A2:G1897"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>